<commit_message>
updated default excel template
changed patient id & diagnosis date in excel file to text
</commit_message>
<xml_diff>
--- a/src/assets/tcia-submission-template.xlsx
+++ b/src/assets/tcia-submission-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliefrund/JavaPrograms/CTP/ROOT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliefrund/Documents/Projects/tcia-submission-vue/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Local Patient ID</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Diagnosis Date (M/D/YYYY)</t>
+  </si>
+  <si>
+    <t>2/3/2008</t>
+  </si>
+  <si>
+    <t>4/9/2007</t>
+  </si>
+  <si>
+    <t>3/31/2017</t>
   </si>
 </sst>
 </file>
@@ -101,9 +110,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,33 +391,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -416,12 +424,12 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>12341234</v>
       </c>
       <c r="B3" t="s">
@@ -430,12 +438,13 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1">
-        <v>39481</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>7980790</v>
       </c>
       <c r="B4" t="s">
@@ -444,12 +453,13 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1">
-        <v>39181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>12348975</v>
       </c>
       <c r="B5" t="s">
@@ -458,12 +468,13 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1">
-        <v>42825</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>13497812</v>
       </c>
       <c r="B6" t="s">
@@ -472,9 +483,10 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1">
-        <v>42825</v>
-      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>